<commit_message>
Add block column in test case and fix something wrong
</commit_message>
<xml_diff>
--- a/v1/test_case_v1.xlsx
+++ b/v1/test_case_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeonbeomgu/Desktop/Seneca College/First Semester/CPR 101/CPR101-Final/v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F605507B-0154-0D40-9A54-5E3EC2535D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF66BC4-7E36-704C-A1D6-50DDB603630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19580" xr2:uid="{201C86A6-83D5-F743-8231-F85975105892}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="27360" xr2:uid="{201C86A6-83D5-F743-8231-F85975105892}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="113">
   <si>
     <t>PASS</t>
   </si>
@@ -353,13 +353,60 @@
   </si>
   <si>
     <t>Main Version 1</t>
+  </si>
+  <si>
+    <t>Indexing</t>
+  </si>
+  <si>
+    <t>Concatenation</t>
+  </si>
+  <si>
+    <t>BLOCK</t>
+  </si>
+  <si>
+    <t>Tokenizing Words</t>
+  </si>
+  <si>
+    <t>Coverting to int</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>TM-V1-06</t>
+  </si>
+  <si>
+    <t>MM-V1-06</t>
+  </si>
+  <si>
+    <t>Type the empty word and "abc"</t>
+  </si>
+  <si>
+    <t>"abc" will be printed</t>
+  </si>
+  <si>
+    <t>"Concatenated string is 'abc'"</t>
+  </si>
+  <si>
+    <t>Type the three word with two space
+CPR class is</t>
+  </si>
+  <si>
+    <t>CPR
+class
+is</t>
+  </si>
+  <si>
+    <t>"Word #1 is 'CPR'
+Word #2 is 'class'
+Word #3 is 'is'"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -417,8 +464,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -449,8 +511,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -713,6 +781,142 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -724,7 +928,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -841,6 +1045,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -853,16 +1069,87 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1210,211 +1497,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65531416-6F40-844D-BFAB-75E18A4BA7BF}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="23"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16" customHeight="1">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="2:9" ht="17" thickBot="1"/>
+    <row r="2" spans="2:9" ht="16" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="17" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="2:9" ht="17" thickBot="1">
+      <c r="B3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" ht="17" thickBot="1"/>
-    <row r="5" spans="2:8" ht="16" customHeight="1" thickBot="1">
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" ht="17" thickBot="1"/>
+    <row r="5" spans="2:9" ht="16" customHeight="1" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="48" customHeight="1">
+    <row r="6" spans="2:9" ht="48" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="48" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="48" customHeight="1">
       <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="48" customHeight="1">
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="48" customHeight="1">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="48" customHeight="1">
+      <c r="I8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="48" customHeight="1">
       <c r="B9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="48" customHeight="1">
+      <c r="I9" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="48" customHeight="1">
       <c r="B10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="48" customHeight="1" thickBot="1">
+      <c r="I10" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="48" customHeight="1" thickBot="1">
       <c r="B11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="G11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1422,211 +1733,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10E8C0E-2D36-9845-8221-F2A2F0150622}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="23"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16" customHeight="1">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="17" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1">
+      <c r="B3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" ht="17" thickBot="1"/>
-    <row r="5" spans="2:8" ht="16" customHeight="1" thickBot="1">
-      <c r="B5" s="3" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1"/>
+    <row r="5" spans="1:9" s="59" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="48" customHeight="1">
+    <row r="6" spans="1:9" ht="48" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="48" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48" customHeight="1">
       <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="48" customHeight="1">
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="48" customHeight="1">
       <c r="B8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="48" customHeight="1">
+    <row r="9" spans="1:9" ht="48" customHeight="1">
       <c r="B9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="72" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="48" customHeight="1">
+    <row r="10" spans="1:9" ht="48" customHeight="1">
       <c r="B10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="48" customHeight="1" thickBot="1">
+    <row r="11" spans="1:9" ht="48" customHeight="1" thickBot="1">
       <c r="B11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="G11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="B2:D3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1635,188 +1971,234 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD68561-A2A3-2D4B-83FA-2F61CFF251CD}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="23"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16" customHeight="1">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="17" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1">
+      <c r="B3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" ht="17" thickBot="1"/>
-    <row r="5" spans="2:8" ht="16" customHeight="1" thickBot="1">
-      <c r="B5" s="3" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1"/>
+    <row r="5" spans="1:9" s="59" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="48" customHeight="1">
+    <row r="6" spans="1:9" ht="48" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="48" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48" customHeight="1">
       <c r="B7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="70">
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="70">
       <c r="B8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="56">
+    <row r="9" spans="1:9" ht="56">
       <c r="B9" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="F9" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="48" customHeight="1" thickBot="1">
-      <c r="B10" s="20" t="s">
+    <row r="10" spans="1:9" ht="48" customHeight="1">
+      <c r="B10" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="65"/>
+    </row>
+    <row r="11" spans="1:9" ht="48" customHeight="1" thickBot="1">
+      <c r="B11" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="G11" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1825,234 +2207,262 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC746E7-EE3E-9A4F-9590-CB964EECDD65}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="23"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16" customHeight="1">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="17" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1">
+      <c r="B3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" ht="17" thickBot="1"/>
-    <row r="5" spans="2:8" ht="16" customHeight="1" thickBot="1">
-      <c r="B5" s="3" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1"/>
+    <row r="5" spans="1:9" s="59" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="48" customHeight="1">
+    <row r="6" spans="1:9" ht="48" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="E6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="48" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48" customHeight="1">
       <c r="B7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="48" customHeight="1">
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="48" customHeight="1">
       <c r="B8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="E8" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="48" customHeight="1">
+      <c r="I8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="48" customHeight="1">
       <c r="B9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="E9" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="48" customHeight="1">
+    <row r="10" spans="1:9" ht="48" customHeight="1">
       <c r="B10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="E10" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="48" customHeight="1">
+    <row r="11" spans="1:9" ht="48" customHeight="1">
       <c r="B11" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="E11" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="F11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="48" customHeight="1" thickBot="1">
+    <row r="12" spans="1:9" ht="48" customHeight="1" thickBot="1">
       <c r="B12" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="E12" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="F12" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="35" t="s">
-        <v>84</v>
-      </c>
       <c r="G12" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="I12" s="36" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2061,188 +2471,236 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C61940-897C-684F-AE72-3CFA8B5A1326}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="1.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="23"/>
-    <col min="8" max="8" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="60.83203125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="23"/>
+    <col min="9" max="9" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17" thickBot="1"/>
-    <row r="2" spans="2:8" ht="16" customHeight="1">
-      <c r="B2" s="44" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1"/>
+    <row r="2" spans="1:9" ht="16" customHeight="1">
+      <c r="B2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="24"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="17" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="17" thickBot="1">
+      <c r="B3" s="42"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="24"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" ht="17" thickBot="1"/>
-    <row r="5" spans="2:8" ht="16" customHeight="1" thickBot="1">
-      <c r="B5" s="3" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1"/>
+    <row r="5" spans="1:9" s="59" customFormat="1" ht="16" customHeight="1" thickBot="1">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="58" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="48" customHeight="1">
+    <row r="6" spans="1:9" ht="48" customHeight="1">
       <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="E6" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="F6" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="48" customHeight="1">
+      <c r="I6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="48" customHeight="1">
       <c r="B7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="48" customHeight="1">
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="48" customHeight="1">
       <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="56">
-      <c r="B9" s="15" t="s">
+      <c r="I8" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="48" customHeight="1">
+      <c r="B9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="48" customHeight="1">
+      <c r="B10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="E10" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F10" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="25" t="s">
+      <c r="G10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I10" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="48" customHeight="1" thickBot="1">
-      <c r="B10" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="33" t="s">
+    <row r="11" spans="1:9" ht="48" customHeight="1" thickBot="1">
+      <c r="B11" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="E11" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="F11" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="35" t="s">
+      <c r="G11" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="I11" s="36" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>